<commit_message>
Add list of the newest products, best seller products and hightest view products
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BC1FCB-5D03-4F3B-ADCC-F687ED5756F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647F8971-EEE1-414E-8069-AF7C33CD7552}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Máy Ảnh Canon EOS 3000D + Lens EF-S 18 - 55mm III (Lê Bảo Minh)</t>
   </si>
@@ -236,13 +236,45 @@
   </si>
   <si>
     <t>DSLR</t>
+  </si>
+  <si>
+    <t>Selfie Lấy Liền Fujifilm Instax Mini 70 - Đỏ</t>
+  </si>
+  <si>
+    <t>Selfie Lấy Liền Fujifilm Instax Mini 70 - Vàng</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>2.690.000 ₫</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.690.000 ₫</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +308,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="13">
@@ -416,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -427,42 +474,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,15 +528,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -815,359 +873,379 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="26" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="B26" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B29" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C29" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14" t="s">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14" t="s">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C31" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14" t="s">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14" t="s">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C33" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14" t="s">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C34" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14" t="s">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14" t="s">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C36" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D36" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1175,10 +1253,10 @@
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A16:A25"/>
-    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A29:A36"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[AdminPage]Create form of admin's information and account
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647F8971-EEE1-414E-8069-AF7C33CD7552}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D654A4-37FF-447A-B0F8-AD56A94FDAE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,11 +316,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
@@ -504,6 +499,16 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -528,17 +533,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -884,7 +879,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -894,7 +889,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="18" t="s">
         <v>65</v>
       </c>
       <c r="H2" s="13" t="s">
@@ -902,7 +897,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -910,13 +905,13 @@
         <v>56</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="G3" s="14"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -924,13 +919,13 @@
         <v>55</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="G4" s="14"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -938,13 +933,13 @@
         <v>54</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="G5" s="14"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -954,7 +949,7 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -964,7 +959,7 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -974,13 +969,13 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -992,7 +987,7 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +997,7 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
@@ -1012,7 +1007,7 @@
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1022,7 +1017,7 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1032,13 +1027,13 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1050,7 +1045,7 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1055,7 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="8" t="s">
         <v>19</v>
       </c>
@@ -1070,7 +1065,7 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
@@ -1080,7 +1075,7 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1090,7 +1085,7 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
@@ -1100,7 +1095,7 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="8" t="s">
         <v>27</v>
       </c>
@@ -1110,7 +1105,7 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
@@ -1120,7 +1115,7 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
@@ -1130,7 +1125,7 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="8" t="s">
         <v>43</v>
       </c>
@@ -1140,33 +1135,33 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="23"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D27" s="15"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -1178,7 +1173,7 @@
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="10" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +1183,7 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="10" t="s">
         <v>33</v>
       </c>
@@ -1198,7 +1193,7 @@
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="10" t="s">
         <v>35</v>
       </c>
@@ -1208,7 +1203,7 @@
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="10" t="s">
         <v>36</v>
       </c>
@@ -1218,7 +1213,7 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="10" t="s">
         <v>37</v>
       </c>
@@ -1228,7 +1223,7 @@
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="10" t="s">
         <v>39</v>
       </c>
@@ -1238,7 +1233,7 @@
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="10" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
[AdminPage]Insert info of all products. Create Add new product form
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9534964F-00F3-4D00-91CD-07B3CA1A0D83}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9120FE12-DE3A-4DD2-AADF-0333BA12B7E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>Máy Ảnh Canon EOS 3000D + Lens EF-S 18 - 55mm III (Lê Bảo Minh)</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>Máy ảnh lấy liền</t>
+  </si>
+  <si>
+    <t>Cơ</t>
+  </si>
+  <si>
+    <t>Kỹ thuật số</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -451,11 +457,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -463,9 +506,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -494,12 +534,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -516,9 +550,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,6 +560,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -847,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -865,388 +917,452 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="G2" s="19" t="s">
+      <c r="D2" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="13" t="s">
+      <c r="D3" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="13" t="s">
+      <c r="D4" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="13"/>
+      <c r="D5" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="23" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="23" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="23" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="25" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="25" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="28"/>
+      <c r="B17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="26" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="28"/>
+      <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="26" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="28"/>
+      <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="26" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="28"/>
+      <c r="B24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="26" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="28"/>
+      <c r="B26" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="15"/>
+      <c r="D26" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="15"/>
+      <c r="D27" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="24" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="10" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="10" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="10" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="10" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="10" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A25"/>
     <mergeCell ref="A29:A36"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A16:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[AdminPage]Add view orders history functionality and Show admin's account information
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9120FE12-DE3A-4DD2-AADF-0333BA12B7E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AA4C38-F1C1-4CF3-97A8-E0672A925704}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[UserPages]Create payment page. [HomePage]Insert information of products
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AA4C38-F1C1-4CF3-97A8-E0672A925704}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E00EAF6-D9EB-4110-98B6-03BABB2836BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
   <si>
     <t>Máy Ảnh Canon EOS 3000D + Lens EF-S 18 - 55mm III (Lê Bảo Minh)</t>
   </si>
@@ -272,12 +272,96 @@
   <si>
     <t>Kỹ thuật số</t>
   </si>
+  <si>
+    <t>Máy Ảnh Canon Powershot G5X (Lê Bảo Minh)</t>
+  </si>
+  <si>
+    <t>13.990.000</t>
+  </si>
+  <si>
+    <t>Canon 5D MARK III + EF 24-105mm F/4 IS</t>
+  </si>
+  <si>
+    <t>59.990.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Canon EOS M100 KIT 15-45mm</t>
+  </si>
+  <si>
+    <t>12.690.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Canon 80D + Lens 18-55mm</t>
+  </si>
+  <si>
+    <t>23.690.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Selfie Lấy Liền Fujifilm Instax Mini 9 - Smoky White</t>
+  </si>
+  <si>
+    <t>1.690.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Fujifilm X-T2 (Body)</t>
+  </si>
+  <si>
+    <t>35.990.000</t>
+  </si>
+  <si>
+    <t>áy Ảnh Fujifilm X-T20 (24.3MP) + Lens 16-50mm - Hàng Chính Hãng</t>
+  </si>
+  <si>
+    <t>21.990.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Selfie Lấy Liền Fujifilm Instax Mini 70 - Xanh</t>
+  </si>
+  <si>
+    <t>2.690.000 </t>
+  </si>
+  <si>
+    <t>Máy Ảnh Selfie Lấy Liền Fujifilm Instax Mini 70 - Vàng Đồng</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Selfie Lấy Liền Fujifilm Instax Mini 70 - Đen</t>
+  </si>
+  <si>
+    <t>2.690.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Fujifilm X-E3 Lens 18-55mm</t>
+  </si>
+  <si>
+    <t>27.590.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Lấy Liền Fujifilm Instax 25</t>
+  </si>
+  <si>
+    <t>2.600.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Nikon D610</t>
+  </si>
+  <si>
+    <t>26.050.000</t>
+  </si>
+  <si>
+    <t>Máy Ảnh Nikon D7500 Body (VIC Nikon)</t>
+  </si>
+  <si>
+    <t>27.990.000</t>
+  </si>
+  <si>
+    <t>Tình trạng đơn hàng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,8 +406,18 @@
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF3425"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +490,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -498,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -562,18 +668,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,6 +676,20 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,19 +1005,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="65.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="5" max="5" width="24.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
@@ -926,6 +1035,9 @@
       <c r="D1" s="11" t="s">
         <v>64</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -937,8 +1049,11 @@
       <c r="C2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="29" t="s">
         <v>73</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>65</v>
@@ -955,8 +1070,11 @@
       <c r="C3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>74</v>
+      <c r="D3" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="12" t="s">
@@ -971,8 +1089,11 @@
       <c r="C4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>74</v>
+      <c r="D4" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="12" t="s">
@@ -987,8 +1108,11 @@
       <c r="C5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>74</v>
+      <c r="D5" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="12"/>
@@ -1001,8 +1125,11 @@
       <c r="C6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>74</v>
+      <c r="D6" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
@@ -1013,356 +1140,542 @@
       <c r="C7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D12" s="29" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="5" t="s">
+      <c r="D14" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D15" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="5" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D16" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="5" t="s">
+      <c r="D17" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D20" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D22" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="7" t="s">
+    <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D23" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="7" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="7" t="s">
+      <c r="D24" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D25" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="7" t="s">
+    <row r="26" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D26" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="7" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="7" t="s">
+      <c r="D27" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D28" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="7" t="s">
+    <row r="29" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="7" t="s">
+      <c r="D29" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="7" t="s">
+      <c r="D30" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D31" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="13" t="s">
+    <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="B32" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C32" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D32" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
-      <c r="B27" s="13" t="s">
+    <row r="33" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
+      <c r="B34" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="24"/>
+      <c r="B36" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="25"/>
+      <c r="B41" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C41" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D41" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C43" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D43" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="9" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="9" t="s">
+      <c r="D44" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C45" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="9" t="s">
+      <c r="D45" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C46" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="9" t="s">
+      <c r="D46" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="9" t="s">
+      <c r="D47" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="9" t="s">
+      <c r="D48" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C49" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="9" t="s">
+      <c r="D49" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="B50" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D50" s="30" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="G2:G5"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A22:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[PaymentPage]Create form of information and total payment of an order
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E00EAF6-D9EB-4110-98B6-03BABB2836BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A657847-E2DC-4678-9D7F-F96E9AEBAE9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -647,36 +647,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -690,6 +660,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1049,13 +1049,13 @@
       <c r="C2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="19" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="1">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="22" t="s">
         <v>65</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -1063,69 +1063,69 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E6" s="1">
@@ -1133,14 +1133,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E7" s="1">
@@ -1148,29 +1148,29 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E8" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="26" t="s">
+    <row r="9" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="20" t="s">
         <v>74</v>
       </c>
       <c r="E9" s="1">
@@ -1178,29 +1178,29 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="19" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="26" t="s">
+    <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="19" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="1">
@@ -1208,14 +1208,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="19" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="1">
@@ -1223,13 +1223,13 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1238,90 +1238,90 @@
       <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+    <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="26" t="s">
+    <row r="19" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="29" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1330,246 +1330,246 @@
       <c r="C22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="D24" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
       <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="26" t="s">
+    <row r="33" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="30"/>
+      <c r="B33" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
-      <c r="B34" s="26" t="s">
+      <c r="A34" s="30"/>
+      <c r="B34" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
-      <c r="B35" s="26" t="s">
+      <c r="D34" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
+      <c r="B35" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="26" t="s">
+      <c r="A36" s="30"/>
+      <c r="B36" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="26" t="s">
+    <row r="37" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="30"/>
+      <c r="B37" s="16" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="26" t="s">
+      <c r="A38" s="30"/>
+      <c r="B38" s="16" t="s">
         <v>92</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="24"/>
-      <c r="B39" s="26" t="s">
+    <row r="39" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="30"/>
+      <c r="B39" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
-      <c r="B40" s="26" t="s">
+    <row r="40" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="30"/>
+      <c r="B40" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="25"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="22"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -1578,91 +1578,91 @@
       <c r="C43" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
+      <c r="D44" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
       <c r="B45" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="D45" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="25"/>
       <c r="B46" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="D49" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="25"/>
       <c r="B50" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="20" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[HomePage] Inserting information of products
</commit_message>
<xml_diff>
--- a/assets/ProductsInfo.xlsx
+++ b/assets/ProductsInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyRepositories\Git\TeamWorkPrograms\1512012_1512013\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A657847-E2DC-4678-9D7F-F96E9AEBAE9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B143822-E699-4024-865C-9D9A7A341F38}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{7FC2539B-84A1-45CB-BC2F-CF565FDC9752}"/>
   </bookViews>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDACA2-5D8B-457F-808F-F31C7F9365E5}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>